<commit_message>
feat(toolbox): integrate Taylor rule model with real DB data
</commit_message>
<xml_diff>
--- a/docs/US Economic Indicators with FRED Codes.xlsx
+++ b/docs/US Economic Indicators with FRED Codes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="186">
   <si>
     <r>
       <rPr>
@@ -372,6 +372,41 @@
         <rFont val="等线"/>
         <charset val="134"/>
       </rPr>
+      <t>自然失业率（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>CBO NAIRU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>Natural Rate of Unemployment (CBO)</t>
+  </si>
+  <si>
+    <t>NROU</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+      </rPr>
       <t>季调各类型失业率</t>
     </r>
   </si>
@@ -458,10 +493,16 @@
     <t>EMRATIO</t>
   </si>
   <si>
-    <t>CPI</t>
-  </si>
-  <si>
-    <r>
+    <t>通胀</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>CPI</t>
     </r>
     <r>
@@ -507,6 +548,15 @@
     <t>CPILFESL</t>
   </si>
   <si>
+    <t>核心PCE同比</t>
+  </si>
+  <si>
+    <t>PCE Price Index Excluding Food and Energy (YoY)</t>
+  </si>
+  <si>
+    <t>PCEPILFE</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -967,6 +1017,57 @@
   </si>
   <si>
     <t>CUSR0000SAS4</t>
+  </si>
+  <si>
+    <t>政策利率</t>
+  </si>
+  <si>
+    <t>有效联邦基金利率</t>
+  </si>
+  <si>
+    <t>Effective Federal Funds Rate</t>
+  </si>
+  <si>
+    <t>EFFR</t>
+  </si>
+  <si>
+    <t>联邦基金目标区间下限</t>
+  </si>
+  <si>
+    <t>Federal Funds Target Range - Lower Limit</t>
+  </si>
+  <si>
+    <t>DFEDTARL</t>
+  </si>
+  <si>
+    <t>联邦基金目标区间上限</t>
+  </si>
+  <si>
+    <t>Federal Funds Target Range - Upper Limit</t>
+  </si>
+  <si>
+    <t>DFEDTARU</t>
+  </si>
+  <si>
+    <t>产出/增长</t>
+  </si>
+  <si>
+    <t>实际GDP</t>
+  </si>
+  <si>
+    <t>Real GDPC1</t>
+  </si>
+  <si>
+    <t>GDPC1</t>
+  </si>
+  <si>
+    <t>潜在GDP</t>
+  </si>
+  <si>
+    <t>Potential GDPPOT</t>
+  </si>
+  <si>
+    <t>GDPPOT</t>
   </si>
 </sst>
 </file>
@@ -979,7 +1080,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,6 +1099,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1513,137 +1620,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1658,22 +1765,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1994,10 +2103,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85"/>
@@ -2037,183 +2146,183 @@
       </c>
     </row>
     <row r="3" ht="13.9" spans="1:4">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" ht="13.9" spans="1:4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="13.9" spans="1:4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="13.9" spans="1:4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" ht="13.9" spans="1:4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" ht="13.9" spans="1:4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" ht="13.9" spans="1:4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" ht="13.9" spans="1:4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" ht="13.9" spans="1:4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" ht="13.9" spans="1:4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" ht="13.9" spans="1:4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" ht="13.9" spans="1:4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" ht="13.9" spans="1:4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" ht="13.9" spans="1:4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" ht="13.9" spans="1:9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
+    <row r="17" ht="13.9" spans="1:4">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" ht="13.9" spans="1:9">
-      <c r="A18" s="5"/>
+    <row r="18" ht="13.9" spans="1:4">
+      <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>51</v>
       </c>
@@ -2224,478 +2333,565 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" ht="13.9" spans="1:9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4" t="s">
+    <row r="19" ht="13.9" spans="1:4">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" ht="13.9" spans="1:4">
+      <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="5"/>
+    <row r="25" spans="1:4">
+      <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" ht="13.9" spans="1:9">
-      <c r="A26" s="5"/>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" ht="13.9" spans="1:9">
-      <c r="A27" s="5"/>
+    <row r="27" ht="13.9" spans="1:4">
+      <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" ht="13.9" spans="1:9">
-      <c r="A28" s="4" t="s">
+    <row r="28" ht="13.9" spans="1:4">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="4" t="s">
+    </row>
+    <row r="29" ht="13.9" spans="1:4">
+      <c r="A29" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" ht="13.9" spans="1:9">
-      <c r="A29" s="5"/>
       <c r="B29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" ht="13.9" spans="1:9">
-      <c r="A30" s="5"/>
+    <row r="30" ht="13.9" spans="1:4">
+      <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" ht="13.9" spans="1:9">
-      <c r="A31" s="5"/>
-      <c r="B31" s="8" t="s">
+      <c r="C30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="8" t="s">
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4"/>
+      <c r="B31" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" ht="13.9" spans="1:9">
-      <c r="A32" s="5"/>
-      <c r="B32" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D31" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="8" t="s">
+    </row>
+    <row r="32" ht="13.9" spans="1:4">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" ht="13.9" spans="1:9">
-      <c r="A33" s="5"/>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="4"/>
+      <c r="B33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" ht="13.9" spans="1:9">
-      <c r="A34" s="5"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="4"/>
+      <c r="B34" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>96</v>
       </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" ht="13.9" spans="1:9">
-      <c r="A35" s="5"/>
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="4"/>
+      <c r="B35" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="6" t="s">
         <v>99</v>
       </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" ht="13.9" spans="1:9">
-      <c r="A36" s="5"/>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="4"/>
+      <c r="B36" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="37" ht="13.9" spans="1:9">
-      <c r="A37" s="5"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="4"/>
+      <c r="B37" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="38" ht="13.9" spans="1:9">
-      <c r="A38" s="5"/>
-      <c r="B38" s="8" t="s">
+      <c r="A38" s="4"/>
+      <c r="B38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="39" ht="13.9" spans="1:9">
-      <c r="A39" s="5"/>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="4"/>
+      <c r="B39" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="40" ht="13.9" spans="1:9">
-      <c r="A40" s="5"/>
-      <c r="B40" s="8" t="s">
+      <c r="A40" s="4"/>
+      <c r="B40" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" ht="13.9" spans="1:9">
-      <c r="A41" s="5"/>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="4"/>
+      <c r="B41" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="42" ht="13.9" spans="1:9">
-      <c r="A42" s="5"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="4"/>
+      <c r="B42" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="43" ht="13.9" spans="1:9">
-      <c r="A43" s="5"/>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="4"/>
+      <c r="B43" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="44" ht="13.9" spans="1:9">
-      <c r="A44" s="5"/>
-      <c r="B44" s="8" t="s">
+      <c r="A44" s="4"/>
+      <c r="B44" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" ht="13.9" spans="1:9">
-      <c r="A45" s="5"/>
-      <c r="B45" s="8" t="s">
+      <c r="A45" s="4"/>
+      <c r="B45" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="6" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="46" ht="13.9" spans="1:9">
-      <c r="A46" s="5"/>
-      <c r="B46" s="8" t="s">
+      <c r="A46" s="4"/>
+      <c r="B46" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="47" ht="13.9" spans="1:9">
-      <c r="A47" s="5"/>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="4"/>
+      <c r="B47" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="6" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="48" ht="13.9" spans="1:9">
-      <c r="A48" s="5"/>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="4"/>
+      <c r="B48" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="6" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="49" ht="13.9" spans="1:4">
-      <c r="A49" s="5"/>
-      <c r="B49" s="8" t="s">
+      <c r="A49" s="4"/>
+      <c r="B49" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="6" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="50" ht="13.9" spans="1:4">
-      <c r="A50" s="5"/>
-      <c r="B50" s="8" t="s">
+      <c r="A50" s="4"/>
+      <c r="B50" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="51" ht="13.9" spans="1:4">
-      <c r="A51" s="5"/>
-      <c r="B51" s="8" t="s">
+      <c r="A51" s="4"/>
+      <c r="B51" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="52" ht="13.9" spans="1:4">
-      <c r="A52" s="5"/>
-      <c r="B52" s="8" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="53" ht="13.9" spans="1:4">
-      <c r="A53" s="5"/>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="4"/>
+      <c r="B53" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="6" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="54" ht="13.9" spans="1:4">
-      <c r="A54" s="5"/>
-      <c r="B54" s="8" t="s">
+      <c r="A54" s="4"/>
+      <c r="B54" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="6" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="55" ht="13.9" spans="1:4">
-      <c r="A55" s="5"/>
-      <c r="B55" s="8" t="s">
+      <c r="A55" s="4"/>
+      <c r="B55" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="6" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="56" ht="13.9" spans="1:4">
-      <c r="A56" s="5"/>
-      <c r="B56" s="8" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="B57" s="1"/>
+    <row r="57" ht="13.9" spans="1:4">
+      <c r="A57" s="4"/>
+      <c r="B57" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" ht="13.9" spans="1:4">
+      <c r="A58" s="4"/>
+      <c r="B58" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="12"/>
+      <c r="B60" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="12"/>
+      <c r="B61" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="12"/>
+      <c r="B63" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A2:A27"/>
-    <mergeCell ref="A28:A56"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A2:A28"/>
+    <mergeCell ref="A29:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>